<commit_message>
debug view working and backlog updated
</commit_message>
<xml_diff>
--- a/WorkProducts/Backlog.xlsx
+++ b/WorkProducts/Backlog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="61">
   <si>
     <t>ID</t>
   </si>
@@ -52,9 +52,6 @@
     <t>Player Component</t>
   </si>
   <si>
-    <t>User moves character, which can jump and interact with other objects.</t>
-  </si>
-  <si>
     <t>Category</t>
   </si>
   <si>
@@ -100,18 +97,6 @@
     <t>Create introduction scene.</t>
   </si>
   <si>
-    <t>Text</t>
-  </si>
-  <si>
-    <t>Text Component</t>
-  </si>
-  <si>
-    <t>User sees text on display.</t>
-  </si>
-  <si>
-    <t>Implement TextComponent.</t>
-  </si>
-  <si>
     <t>User sees NPCs acting on needs and according to different moods (levels of aggression).</t>
   </si>
   <si>
@@ -167,6 +152,51 @@
   </si>
   <si>
     <t>Implement interaction system for all of the Sprint 1 components so that their effects combine and stack appropriately.</t>
+  </si>
+  <si>
+    <t>User moves character, which can jump and walk on surfaces.</t>
+  </si>
+  <si>
+    <t>Graphics</t>
+  </si>
+  <si>
+    <t>Light</t>
+  </si>
+  <si>
+    <t>User sees lights emitted from game objects.</t>
+  </si>
+  <si>
+    <t>Implement lighting scheme.</t>
+  </si>
+  <si>
+    <t>Implementation Plan</t>
+  </si>
+  <si>
+    <t>Use Farseer Physics Engine.</t>
+  </si>
+  <si>
+    <t>Use InputHelper class (still need to make modifications to the class).</t>
+  </si>
+  <si>
+    <t>Create a player component that can draw itself, and add a physics component that keeps track of position for the drawing.</t>
+  </si>
+  <si>
+    <t>Create a shadow image for each object emitting light that shows a black/white representation of the lighting in the scene that takes into account the effect of other objects in the scene creating shadows. Then, blend them all together with the appropriate colors and display this information on the background, which will create a dynamic 2D lighting effect.</t>
+  </si>
+  <si>
+    <t>PhysicsComponent</t>
+  </si>
+  <si>
+    <t>Game object has appropriate physics.</t>
+  </si>
+  <si>
+    <t>Implement PhysicsComponent.</t>
+  </si>
+  <si>
+    <t>The physics component should be re-usable, and will be backed by the Farseer engine. Basically, this component should contain Fixture information/variables, so we always have the position in the physics world of each object that has this physics component. Then other components can retrieve the position of the Fixture's Body variable.</t>
+  </si>
+  <si>
+    <t>Attach lighting and physics components to a light object. Then, check the game world to see which objects are in the light given by the light component, and apply upward force to each object until the light is no longer touching the objects.</t>
   </si>
 </sst>
 </file>
@@ -515,30 +545,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.5546875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="94" style="4" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.21875" style="4" customWidth="1"/>
     <col min="5" max="5" width="27.88671875" style="4" customWidth="1"/>
     <col min="6" max="6" width="9" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="43.21875" customWidth="1"/>
+    <col min="9" max="9" width="15.109375" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
@@ -547,7 +579,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -556,21 +588,24 @@
         <v>4</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="F2" s="1">
         <v>10</v>
@@ -578,245 +613,295 @@
       <c r="G2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H2" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="2">
+        <v>40462</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="1">
+        <v>8</v>
+      </c>
+      <c r="G3" s="1">
+        <v>2</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="I3" s="2">
+        <v>40472</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" s="1">
+        <v>10</v>
+      </c>
+      <c r="G4" s="1">
+        <v>2</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="1">
+        <v>10</v>
+      </c>
+      <c r="G5" s="1">
+        <v>2</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="1">
+        <v>10</v>
+      </c>
+      <c r="G6" s="1">
+        <v>2</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="1">
+        <v>10</v>
+      </c>
+      <c r="G7" s="1">
+        <v>3</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="1">
+        <v>10</v>
+      </c>
+      <c r="G8" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="1">
+        <v>10</v>
+      </c>
+      <c r="G9" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="1">
+        <v>10</v>
+      </c>
+      <c r="G10" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="1">
+        <v>10</v>
+      </c>
+      <c r="G11" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="F3" s="1">
-        <v>10</v>
-      </c>
-      <c r="G3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D4" s="4" t="s">
+      <c r="D12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="F4" s="1">
-        <v>10</v>
-      </c>
-      <c r="G4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="F5" s="1">
-        <v>10</v>
-      </c>
-      <c r="G5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="F6" s="1">
-        <v>10</v>
-      </c>
-      <c r="G6" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F7" s="1">
-        <v>10</v>
-      </c>
-      <c r="G7" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="4" t="s">
+      <c r="F12" s="1">
+        <v>10</v>
+      </c>
+      <c r="G12" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="1">
         <v>7</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="1">
+      <c r="G13" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F9" s="1">
-        <v>10</v>
-      </c>
-      <c r="G9" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="4" t="s">
+      <c r="D14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="1">
-        <v>10</v>
-      </c>
-      <c r="G10" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
+      <c r="F14" s="1">
+        <v>8</v>
+      </c>
+      <c r="G14" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="4" t="s">
+      <c r="C15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" s="1">
         <v>9</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F11" s="1">
-        <v>8</v>
-      </c>
-      <c r="G11" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" s="1">
-        <v>9</v>
-      </c>
-      <c r="G12" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="G13" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F14" s="1">
-        <v>7</v>
-      </c>
-      <c r="G14" s="1">
-        <v>3</v>
+      <c r="G15" s="1">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:I15">
+    <sortCondition ref="G1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated article, added article template, and updated backlog.
</commit_message>
<xml_diff>
--- a/WorkProducts/Backlog.xlsx
+++ b/WorkProducts/Backlog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="71">
   <si>
     <t>ID</t>
   </si>
@@ -209,6 +209,24 @@
   </si>
   <si>
     <t>Create introduction scene.</t>
+  </si>
+  <si>
+    <t>Create a component that provides a multiplier for components to use when deciding the force that is moving them, so that speed can be modified by the light for any object that its touching.</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>3\4</t>
+  </si>
+  <si>
+    <t>MovingPlatformComponent</t>
+  </si>
+  <si>
+    <t>User can utilize a platform that moves between a collection of points with a certain velocity.</t>
+  </si>
+  <si>
+    <t>Create a PhysicsComponent that is pushed from point to point in a list of destinations with application of forces, creating a moving platform.</t>
   </si>
 </sst>
 </file>
@@ -216,7 +234,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="mm/dd/yy;@"/>
+    <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -693,7 +711,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1038,11 +1056,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
+      <selection pane="bottomLeft" activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1252,8 +1270,8 @@
       <c r="F7" s="2">
         <v>10</v>
       </c>
-      <c r="G7" s="2">
-        <v>3</v>
+      <c r="G7" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>35</v>
@@ -1279,7 +1297,7 @@
         <v>10</v>
       </c>
       <c r="G8" s="2">
-        <v>3</v>
+        <v>0.75</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>38</v>
@@ -1304,8 +1322,8 @@
       <c r="F9" s="2">
         <v>10</v>
       </c>
-      <c r="G9" s="2">
-        <v>3</v>
+      <c r="G9" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>42</v>
@@ -1330,6 +1348,9 @@
       <c r="F10" s="2">
         <v>10</v>
       </c>
+      <c r="G10" s="2">
+        <v>4</v>
+      </c>
       <c r="H10" s="4" t="s">
         <v>47</v>
       </c>
@@ -1337,7 +1358,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -1357,7 +1378,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -1375,6 +1396,12 @@
       </c>
       <c r="F12" s="2">
         <v>10</v>
+      </c>
+      <c r="G12" s="2">
+        <v>4</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1435,6 +1462,29 @@
       </c>
       <c r="F15" s="2">
         <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" s="2">
+        <v>10</v>
+      </c>
+      <c r="G16" s="2">
+        <v>4</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding temporary sprint 5 plan.
</commit_message>
<xml_diff>
--- a/WorkProducts/Backlog.xlsx
+++ b/WorkProducts/Backlog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="85">
   <si>
     <t>ID</t>
   </si>
@@ -227,6 +227,48 @@
   </si>
   <si>
     <t>Create a PhysicsComponent that is pushed from point to point in a list of destinations with application of forces, creating a moving platform.</t>
+  </si>
+  <si>
+    <t>Audio</t>
+  </si>
+  <si>
+    <t>AudioComponent</t>
+  </si>
+  <si>
+    <t>User hears music and sound effects.</t>
+  </si>
+  <si>
+    <t>Use XACT and related libraries to implement another component that can be contacted by other components with a message telling the component which sound to play, how to manipulate volume, and other important actions as defined.</t>
+  </si>
+  <si>
+    <t>Configuration</t>
+  </si>
+  <si>
+    <t>Configuration File and Objects.</t>
+  </si>
+  <si>
+    <t>User sees configuration file that can be edited.</t>
+  </si>
+  <si>
+    <t>Impement or integrate a config file system.</t>
+  </si>
+  <si>
+    <t>Integrate EasyConfig and write configuration files for all game data that should be easily tweakable from outside the game.</t>
+  </si>
+  <si>
+    <t>Define introductory level in Tiled and script events.</t>
+  </si>
+  <si>
+    <t>Scripting</t>
+  </si>
+  <si>
+    <t>User sees dynamic and interesting effects, camera movements, etc.</t>
+  </si>
+  <si>
+    <t>Create scripting mechanism.</t>
+  </si>
+  <si>
+    <t>Write a script manager that accepts scripts and plays them in the game world, so that camera movements and effects and sounds can be defined outside the game code. This includes complete cinematic moments in which the user does nothing but watch certain events unfold.</t>
   </si>
 </sst>
 </file>
@@ -1056,11 +1098,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1329,47 +1371,44 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="132.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="F10" s="2">
         <v>10</v>
       </c>
       <c r="G10" s="2">
-        <v>4</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>50</v>
+        <v>73</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>26</v>
@@ -1377,102 +1416,132 @@
       <c r="F11" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="G11" s="2">
+        <v>5</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>23</v>
+        <v>75</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>51</v>
+        <v>76</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>52</v>
+        <v>77</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>26</v>
+        <v>78</v>
       </c>
       <c r="F12" s="2">
         <v>10</v>
       </c>
       <c r="G12" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="F13" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="G13" s="2">
+        <v>5</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>60</v>
+        <v>83</v>
       </c>
       <c r="F14" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="G14" s="2">
+        <v>5</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="132.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="F15" s="2">
+        <v>10</v>
+      </c>
+      <c r="G15" s="2">
+        <v>5</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
         <v>9</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>26</v>
@@ -1481,10 +1550,79 @@
         <v>10</v>
       </c>
       <c r="G16" s="2">
-        <v>4</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>70</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>10</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" s="2">
+        <v>10</v>
+      </c>
+      <c r="G17" s="2">
+        <v>6</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>12</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F18" s="2">
+        <v>7</v>
+      </c>
+      <c r="G18" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>13</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F19" s="2">
+        <v>8</v>
+      </c>
+      <c r="G19" s="2">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Major code overhaul. Added menu system and revised component system.
</commit_message>
<xml_diff>
--- a/WorkProducts/Backlog.xlsx
+++ b/WorkProducts/Backlog.xlsx
@@ -1102,7 +1102,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <selection pane="bottomLeft" activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1397,7 +1397,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>16</v>
       </c>
@@ -1421,6 +1421,9 @@
       </c>
       <c r="H11" s="1" t="s">
         <v>74</v>
+      </c>
+      <c r="I11" s="5">
+        <v>40555</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -1447,6 +1450,9 @@
       </c>
       <c r="H12" s="1" t="s">
         <v>79</v>
+      </c>
+      <c r="I12" s="5">
+        <v>40555</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Got light to work with camera. Just need to implement the rest of the lighting infrastructure now, which is already partially done. Also pulled in DebugViewXNA so that I'm no longer referencing any external projects. Need to clean up comments and other garbage created by trying to get the lights to work.
</commit_message>
<xml_diff>
--- a/WorkProducts/Backlog.xlsx
+++ b/WorkProducts/Backlog.xlsx
@@ -1101,8 +1101,8 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I13" sqref="I13"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1391,7 +1391,7 @@
         <v>10</v>
       </c>
       <c r="G10" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>70</v>
@@ -1475,7 +1475,7 @@
         <v>9</v>
       </c>
       <c r="G13" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>80</v>
@@ -1501,7 +1501,7 @@
         <v>9</v>
       </c>
       <c r="G14" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>84</v>
@@ -1527,7 +1527,7 @@
         <v>10</v>
       </c>
       <c r="G15" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H15" s="4" t="s">
         <v>47</v>

</xml_diff>

<commit_message>
Added bloom classes and working test code for bloom effects.
</commit_message>
<xml_diff>
--- a/WorkProducts/Backlog.xlsx
+++ b/WorkProducts/Backlog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="100">
   <si>
     <t>ID</t>
   </si>
@@ -133,18 +133,6 @@
     <t>Create a LightPlatform class that is created and easily manipulated by a PlatformLight. The LightPlatform class should have a platform variable and be able to move its position, making it a dynamic in the physics world, and should be able to determine the position of the platform in the game world. This calls for a platform class that will make this easy.</t>
   </si>
   <si>
-    <t>Component Interaction</t>
-  </si>
-  <si>
-    <t>Light Component effects can combine to create dynamic light combinations at runtime.</t>
-  </si>
-  <si>
-    <t>Implement interaction system for all of the Sprint 1 components so that their effects combine and stack appropriately.</t>
-  </si>
-  <si>
-    <t>Create a light communication system. A class called something like LightManager should provide easy access to all light fields for all other light fields. This way, they can access properties like LightingEnabled, EffectEnabled, LightDistance, LightBrightness, and so forth. Then all lights will be able to manipulate each other at runtime depending on their circumstances. One idea is to implement the LightEffect with a strategy pattern so that light functions can be easily swapped. This could come in useful when the null light touches other lights, because then at that point the null light could convert the light to its functionality instead of modifying individual light properties. There are reasons I'd want to do both things though, so I don't know how useful utilizing the pattern would be. But it would make changing lights to something entirely different really easy, which is something I'll probably want to do.</t>
-  </si>
-  <si>
     <t>Graphics</t>
   </si>
   <si>
@@ -217,9 +205,6 @@
     <t>?</t>
   </si>
   <si>
-    <t>3\4</t>
-  </si>
-  <si>
     <t>MovingPlatformComponent</t>
   </si>
   <si>
@@ -256,9 +241,6 @@
     <t>Integrate EasyConfig and write configuration files for all game data that should be easily tweakable from outside the game.</t>
   </si>
   <si>
-    <t>Define introductory level in Tiled and script events.</t>
-  </si>
-  <si>
     <t>Scripting</t>
   </si>
   <si>
@@ -269,6 +251,69 @@
   </si>
   <si>
     <t>Write a script manager that accepts scripts and plays them in the game world, so that camera movements and effects and sounds can be defined outside the game code. This includes complete cinematic moments in which the user does nothing but watch certain events unfold.</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Cancelled</t>
+  </si>
+  <si>
+    <t>Player</t>
+  </si>
+  <si>
+    <t>Health</t>
+  </si>
+  <si>
+    <t>User sees player character get hit and the screen is covered by a blur effect whose intensity is related to the amount of player health left.</t>
+  </si>
+  <si>
+    <t>Activate BlurPostProcessing component (already implemented) and tune its intensity according to player health.</t>
+  </si>
+  <si>
+    <t>Activate the post-processing component that is already a part of the project and call its functions at the appropriate time each Draw() so that the post-processing effects are applied to the entire game scene (call it after everything else has been drawn).</t>
+  </si>
+  <si>
+    <t>PlayerControllableLight</t>
+  </si>
+  <si>
+    <t>User uses keys or the right Xbox control stick to aim a light in the direction indicated by the input.</t>
+  </si>
+  <si>
+    <t>Implement an interface to lights that are marked interactive so that player input can be used to manipulate them.</t>
+  </si>
+  <si>
+    <t>Create a new boolean light property that marks whether or not a light is interactive. If the player activates it with a button press or something, then utilize player input to decide which direction the light is facing.</t>
+  </si>
+  <si>
+    <t>Define introductory level in Tiled and script events. Tutorial text can be hidden in the level's darkness and read with a light.</t>
+  </si>
+  <si>
+    <t>Bugs</t>
+  </si>
+  <si>
+    <t>Bug Fixes</t>
+  </si>
+  <si>
+    <t>User does NOT experience bugs.</t>
+  </si>
+  <si>
+    <t>Fix as many bugs logged on GitHub as possible.</t>
+  </si>
+  <si>
+    <t>Fix bugs according to individual bug requirements.</t>
+  </si>
+  <si>
+    <t>Symposium Demo</t>
+  </si>
+  <si>
+    <t>User is able to pick up game and play from any point in the introductory level.</t>
+  </si>
+  <si>
+    <t>Ensure that the symposium demo works as expected on PC and Xbox platforms.</t>
+  </si>
+  <si>
+    <t>Run through symposium demo and have friends test for bugs.</t>
   </si>
 </sst>
 </file>
@@ -1098,10 +1143,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
@@ -1312,25 +1357,28 @@
       <c r="F7" s="2">
         <v>10</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>67</v>
+      <c r="G7" s="2">
+        <v>4</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="I7" s="5">
+        <v>40491</v>
+      </c>
     </row>
     <row r="8" spans="1:9" ht="150" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>23</v>
+        <v>66</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>26</v>
@@ -1339,53 +1387,59 @@
         <v>10</v>
       </c>
       <c r="G8" s="2">
-        <v>0.75</v>
+        <v>5</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="387" customHeight="1" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="I8" s="5">
+        <v>40555</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>39</v>
+        <v>71</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>41</v>
+        <v>73</v>
       </c>
       <c r="F9" s="2">
         <v>10</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>66</v>
+      <c r="G9" s="2">
+        <v>5</v>
       </c>
       <c r="H9" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I9" s="5">
+        <v>40555</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>4</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>15</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>26</v>
       </c>
       <c r="F10" s="2">
         <v>10</v>
@@ -1393,22 +1447,25 @@
       <c r="G10" s="2">
         <v>6</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="H10" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>71</v>
+        <v>23</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>72</v>
+        <v>47</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>73</v>
+        <v>48</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>26</v>
@@ -1417,221 +1474,317 @@
         <v>10</v>
       </c>
       <c r="G11" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="I11" s="5">
-        <v>40555</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>40613</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>75</v>
+        <v>23</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>76</v>
+        <v>36</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>77</v>
+        <v>37</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>78</v>
+        <v>26</v>
       </c>
       <c r="F12" s="2">
         <v>10</v>
       </c>
       <c r="G12" s="2">
+        <v>8</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>15</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="2">
+        <v>10</v>
+      </c>
+      <c r="G13" s="2">
+        <v>8</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>21</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="F14" s="2">
         <v>5</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="I12" s="5">
-        <v>40555</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
+      <c r="G14" s="2">
+        <v>8</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>20</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F15" s="2">
+        <v>8</v>
+      </c>
+      <c r="G15" s="2">
+        <v>8</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
         <v>14</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F13" s="2">
+      <c r="B16" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F16" s="2">
         <v>9</v>
       </c>
-      <c r="G13" s="2">
-        <v>6</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>19</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="F14" s="2">
-        <v>9</v>
-      </c>
-      <c r="G14" s="2">
-        <v>6</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="132.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>4</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F15" s="2">
-        <v>10</v>
-      </c>
-      <c r="G15" s="2">
-        <v>6</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="I15" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <v>9</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F16" s="2">
-        <v>10</v>
-      </c>
       <c r="G16" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>23</v>
+        <v>91</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>52</v>
+        <v>93</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>26</v>
+        <v>94</v>
       </c>
       <c r="F17" s="2">
         <v>10</v>
       </c>
       <c r="G17" s="2">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
+        <v>23</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F18" s="2">
+        <v>10</v>
+      </c>
+      <c r="G18" s="2">
+        <v>9</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>19</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F19" s="2">
+        <v>9</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>9</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" s="2">
+        <v>10</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
         <v>12</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B21" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F21" s="2">
+        <v>7</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>13</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C22" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D22" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E22" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="F18" s="2">
-        <v>7</v>
-      </c>
-      <c r="G18" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <v>13</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="F19" s="2">
+      <c r="F22" s="2">
         <v>8</v>
       </c>
-      <c r="G19" s="2">
-        <v>6</v>
+      <c r="G22" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:I18">
+    <sortCondition ref="G2:G18"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>